<commit_message>
incorpoated API to all services
</commit_message>
<xml_diff>
--- a/DemoApi/output.xlsx
+++ b/DemoApi/output.xlsx
@@ -14,7 +14,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>Overhead (bytes)</t>
+    <t>Document size (bytes)</t>
   </si>
 </sst>
 </file>
@@ -72,7 +72,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>9.0</v>
+        <v>2427.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>